<commit_message>
code optimaization in curl
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelResultsFolder/purchaseResults.xlsx
+++ b/src/test/resources/ExcelResultsFolder/purchaseResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\eclipse-workspace\integrationApiUiTesting\src\test\resources\ExcelResultsFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B2A5A1-F4B8-4600-B7A8-643343FB8B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DA0DA7-6FA6-4641-9EB4-21CE6EEF342D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmailData" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="EmailId_Result" sheetId="22" r:id="rId21"/>
     <sheet name="Zipcode_Result" sheetId="23" r:id="rId22"/>
     <sheet name="EndToEnd_Result" sheetId="24" r:id="rId23"/>
+    <sheet name="CreateCustomerAndSession" sheetId="25" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2296" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="677">
   <si>
     <t>Email</t>
   </si>
@@ -1726,6 +1727,366 @@
   </si>
   <si>
     <t>2025-12-22 12:10:31</t>
+  </si>
+  <si>
+    <t>694931363fbd5815ff04f602</t>
+  </si>
+  <si>
+    <t>2025-12-22 17:24:09</t>
+  </si>
+  <si>
+    <t>INR VISA</t>
+  </si>
+  <si>
+    <t>694931853fbd5815ff04f8c3</t>
+  </si>
+  <si>
+    <t>2025-12-22 17:27:10</t>
+  </si>
+  <si>
+    <t>6949326d3fbd5815ff04fe5b</t>
+  </si>
+  <si>
+    <t>2025-12-22 17:29:20</t>
+  </si>
+  <si>
+    <t>USD MASTER</t>
+  </si>
+  <si>
+    <t>694933e63fbd5815ff05084f</t>
+  </si>
+  <si>
+    <t>2025-12-22 17:36:01</t>
+  </si>
+  <si>
+    <t>6949373a3fbd5815ff05125b</t>
+  </si>
+  <si>
+    <t>2025-12-22 17:50:10</t>
+  </si>
+  <si>
+    <t>6949385f3fbd5815ff0519c8</t>
+  </si>
+  <si>
+    <t>2025-12-22 17:55:04</t>
+  </si>
+  <si>
+    <t>694a21584a4f53f748f9c0c3</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:30:32</t>
+  </si>
+  <si>
+    <t>694a22324a4f53f748f9c4a4</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:34:01</t>
+  </si>
+  <si>
+    <t>694a241c4a4f53f748f9c900</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:42:11</t>
+  </si>
+  <si>
+    <t>694a25304a4f53f748f9ccf0</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:46:47</t>
+  </si>
+  <si>
+    <t>694a25dc4a4f53f748f9d0b8</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:49:37</t>
+  </si>
+  <si>
+    <t>694a26884a4f53f748f9d47f</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:52:39</t>
+  </si>
+  <si>
+    <t>694a273b4a4f53f748f9dafe</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:55:39</t>
+  </si>
+  <si>
+    <t>694a27f14a4f53f748f9dec2</t>
+  </si>
+  <si>
+    <t>2025-12-23 10:58:31</t>
+  </si>
+  <si>
+    <t>694a29154a4f53f748f9e29f</t>
+  </si>
+  <si>
+    <t>2025-12-23 11:03:26</t>
+  </si>
+  <si>
+    <t>694a29cd4a4f53f748f9e65c</t>
+  </si>
+  <si>
+    <t>2025-12-23 11:06:29</t>
+  </si>
+  <si>
+    <t>694a2a824a4f53f748f9ea07</t>
+  </si>
+  <si>
+    <t>2025-12-23 11:09:29</t>
+  </si>
+  <si>
+    <t>694a2b3a4a4f53f748f9edb2</t>
+  </si>
+  <si>
+    <t>2025-12-23 11:12:44</t>
+  </si>
+  <si>
+    <t>694a2bf44a4f53f748f9f167</t>
+  </si>
+  <si>
+    <t>2025-12-23 11:15:41</t>
+  </si>
+  <si>
+    <t>694a2dce4a4f53f748f9f81e</t>
+  </si>
+  <si>
+    <t>2025-12-23 11:21:53</t>
+  </si>
+  <si>
+    <t>CLP VISA</t>
+  </si>
+  <si>
+    <t>694a80076121018246f93d68</t>
+  </si>
+  <si>
+    <t>2025-12-23 17:12:20</t>
+  </si>
+  <si>
+    <t>694a80c36121018246f93fec</t>
+  </si>
+  <si>
+    <t>2025-12-23 17:15:26</t>
+  </si>
+  <si>
+    <t>PEN VISA</t>
+  </si>
+  <si>
+    <t>694a860e6ab547d8d6261e4e</t>
+  </si>
+  <si>
+    <t>2025-12-23 17:38:01</t>
+  </si>
+  <si>
+    <t>694a87136ab547d8d62620db</t>
+  </si>
+  <si>
+    <t>2025-12-23 17:42:23</t>
+  </si>
+  <si>
+    <t>694a8a9ec89ddcf8f3998bec</t>
+  </si>
+  <si>
+    <t>2025-12-23 17:57:34</t>
+  </si>
+  <si>
+    <t>694a8c69c89ddcf8f3999831</t>
+  </si>
+  <si>
+    <t>2025-12-23 18:05:18</t>
+  </si>
+  <si>
+    <t>694a8f18c89ddcf8f399a782</t>
+  </si>
+  <si>
+    <t>2025-12-23 18:16:44</t>
+  </si>
+  <si>
+    <t>694b7ce404f0708ed1e91269</t>
+  </si>
+  <si>
+    <t>2025-12-24 11:11:16</t>
+  </si>
+  <si>
+    <t>694b7d5904f0708ed1e914f1</t>
+  </si>
+  <si>
+    <t>2025-12-24 11:13:11</t>
+  </si>
+  <si>
+    <t>694b812f04f0708ed1e91c62</t>
+  </si>
+  <si>
+    <t>2025-12-24 11:29:37</t>
+  </si>
+  <si>
+    <t>694b813204f0708ed1e91c68</t>
+  </si>
+  <si>
+    <t>2025-12-24 11:29:43</t>
+  </si>
+  <si>
+    <t>694b841204f0708ed1e921fe</t>
+  </si>
+  <si>
+    <t>2025-12-24 11:43:11</t>
+  </si>
+  <si>
+    <t>694b846904f0708ed1e92489</t>
+  </si>
+  <si>
+    <t>2025-12-24 11:45:52</t>
+  </si>
+  <si>
+    <t>MXN VISA</t>
+  </si>
+  <si>
+    <t>694b85e904f0708ed1e92a62</t>
+  </si>
+  <si>
+    <t>2025-12-24 11:49:49</t>
+  </si>
+  <si>
+    <t>07/28</t>
+  </si>
+  <si>
+    <t>Master4105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5553042241984105 </t>
+  </si>
+  <si>
+    <t>2025-12-24 12:16:11</t>
+  </si>
+  <si>
+    <t>694b8c5e04f0708ed1e93568</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:19:21</t>
+  </si>
+  <si>
+    <t>694b8d2404f0708ed1e93856</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:21:10</t>
+  </si>
+  <si>
+    <t>694b8d9204f0708ed1e93b49</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:22:59</t>
+  </si>
+  <si>
+    <t>694b8e0704f0708ed1e93e3c</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:24:58</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:26:03</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:26:22</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:26:47</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:27:09</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:27:29</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:27:50</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:39:45</t>
+  </si>
+  <si>
+    <t>694b931804f0708ed1e94ce2</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:46:26</t>
+  </si>
+  <si>
+    <t>694b940204f0708ed1e9538e</t>
+  </si>
+  <si>
+    <t>2025-12-24 12:50:18</t>
+  </si>
+  <si>
+    <t>694b977204f0708ed1e95dd3</t>
+  </si>
+  <si>
+    <t>2025-12-24 13:04:53</t>
+  </si>
+  <si>
+    <t>694bad18e2188cbf0dda77ca</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:37:18</t>
+  </si>
+  <si>
+    <t>useralias@gmail.com</t>
+  </si>
+  <si>
+    <t>694bad8be2188cbf0dda7a7e</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:39:15</t>
+  </si>
+  <si>
+    <t>694bae29e2188cbf0dda7d39</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:41:54</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:52:20</t>
+  </si>
+  <si>
+    <t>694bb0e3197becacc1a08026</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:53:26</t>
+  </si>
+  <si>
+    <t>694bb143197becacc1a08309</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:55:01</t>
+  </si>
+  <si>
+    <t>694bb1a3197becacc1a085e8</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:56:38</t>
+  </si>
+  <si>
+    <t>694bb205197becacc1a088cd</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:58:16</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:59:15</t>
+  </si>
+  <si>
+    <t>2025-12-24 14:59:37</t>
+  </si>
+  <si>
+    <t>2025-12-24 15:00:09</t>
+  </si>
+  <si>
+    <t>2025-12-24 15:00:32</t>
+  </si>
+  <si>
+    <t>2025-12-24 15:00:55</t>
+  </si>
+  <si>
+    <t>2025-12-24 15:01:23</t>
   </si>
 </sst>
 </file>
@@ -1733,7 +2094,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1810,6 +2171,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF292A2E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1875,7 +2243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1922,6 +2290,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2225,10 +2594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F36" sqref="A26:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2732,6 +3101,223 @@
       </c>
       <c r="F25" s="8" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E26" s="8">
+        <v>123</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E27" s="8">
+        <v>123</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E28" s="8">
+        <v>123</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E29" s="8">
+        <v>123</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E30" s="8">
+        <v>123</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E31" s="8">
+        <v>123</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E32" s="8">
+        <v>123</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E33" s="8">
+        <v>123</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E34" s="8">
+        <v>123</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B35" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E35" s="8">
+        <v>123</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E36" s="8">
+        <v>123</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -4185,7 +4771,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A2:E34"/>
+  <dimension ref="A2:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -4626,6 +5212,465 @@
       </c>
       <c r="E34" t="s" s="0">
         <v>454</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="D35" s="0"/>
+      <c r="E35" t="s" s="0">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>634</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>636</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>638</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>640</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" t="s" s="0">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="D41" s="0"/>
+      <c r="E41" t="s" s="0">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="D42" s="0"/>
+      <c r="E42" t="s" s="0">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="D43" s="0"/>
+      <c r="E43" t="s" s="0">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="D44" s="0"/>
+      <c r="E44" t="s" s="0">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0"/>
+      <c r="B45" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="D45" s="0"/>
+      <c r="E45" t="s" s="0">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="D46" s="0"/>
+      <c r="E46" t="s" s="0">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>649</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>651</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>653</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>655</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>657</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>658</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>657</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>660</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="D53" s="0"/>
+      <c r="E53" t="s" s="0">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>663</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>665</v>
+      </c>
+      <c r="E55" t="s" s="0">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>667</v>
+      </c>
+      <c r="E56" t="s" s="0">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>657</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>669</v>
+      </c>
+      <c r="E57" t="s" s="0">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="D58" s="0"/>
+      <c r="E58" t="s" s="0">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="D59" s="0"/>
+      <c r="E59" t="s" s="0">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="D60" s="0"/>
+      <c r="E60" t="s" s="0">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="D61" s="0"/>
+      <c r="E61" t="s" s="0">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="D62" s="0"/>
+      <c r="E62" t="s" s="0">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0"/>
+      <c r="B63" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="D63" s="0"/>
+      <c r="E63" t="s" s="0">
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -4885,7 +5930,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A2:E26"/>
+  <dimension ref="A2:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -5198,7 +6243,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
         <v>520</v>
       </c>
@@ -5215,7 +6260,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
         <v>21</v>
       </c>
@@ -5232,7 +6277,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
         <v>21</v>
       </c>
@@ -5249,7 +6294,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
         <v>21</v>
       </c>
@@ -5264,6 +6309,91 @@
       </c>
       <c r="E26" t="s" s="0">
         <v>556</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s" s="0">
+        <v>483</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>557</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s" s="0">
+        <v>559</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>560</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s" s="0">
+        <v>483</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>562</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>565</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>567</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -7331,7 +8461,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -7533,7 +8663,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
         <v>483</v>
       </c>
@@ -7550,7 +8680,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
         <v>483</v>
       </c>
@@ -7567,7 +8697,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
         <v>483</v>
       </c>
@@ -7584,7 +8714,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
         <v>483</v>
       </c>
@@ -7601,7 +8731,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
         <v>483</v>
       </c>
@@ -7618,7 +8748,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
         <v>483</v>
       </c>
@@ -7635,7 +8765,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
         <v>483</v>
       </c>
@@ -7652,7 +8782,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
         <v>483</v>
       </c>
@@ -7669,7 +8799,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
         <v>483</v>
       </c>
@@ -7686,7 +8816,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
         <v>483</v>
       </c>
@@ -7703,7 +8833,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
         <v>483</v>
       </c>
@@ -7720,7 +8850,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
         <v>483</v>
       </c>
@@ -7737,7 +8867,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
         <v>483</v>
       </c>
@@ -7754,7 +8884,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
         <v>483</v>
       </c>
@@ -7771,7 +8901,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
         <v>483</v>
       </c>
@@ -7788,7 +8918,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
         <v>483</v>
       </c>
@@ -7805,7 +8935,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
         <v>483</v>
       </c>
@@ -7822,7 +8952,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
         <v>376</v>
       </c>
@@ -7839,7 +8969,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
         <v>483</v>
       </c>
@@ -7856,7 +8986,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
         <v>483</v>
       </c>
@@ -7873,7 +9003,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
         <v>483</v>
       </c>
@@ -7890,7 +9020,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s" s="0">
         <v>483</v>
       </c>
@@ -7907,7 +9037,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
         <v>483</v>
       </c>
@@ -7924,7 +9054,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
         <v>483</v>
       </c>
@@ -7941,7 +9071,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
         <v>483</v>
       </c>
@@ -7958,7 +9088,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
         <v>483</v>
       </c>
@@ -7975,7 +9105,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
         <v>483</v>
       </c>
@@ -7992,7 +9122,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
         <v>483</v>
       </c>
@@ -8009,7 +9139,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
         <v>483</v>
       </c>
@@ -8026,7 +9156,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
         <v>483</v>
       </c>
@@ -8043,7 +9173,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
         <v>483</v>
       </c>
@@ -8060,7 +9190,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
         <v>483</v>
       </c>
@@ -8075,6 +9205,538 @@
       </c>
       <c r="E43" t="s" s="0">
         <v>550</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s" s="0">
+        <v>599</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>600</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s" s="0">
+        <v>599</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>602</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>605</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>607</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>609</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>611</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>613</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>615</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>617</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>619</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>621</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>623</v>
+      </c>
+      <c r="E55" t="s" s="0">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s" s="0">
+        <v>599</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>625</v>
+      </c>
+      <c r="E56" t="s" s="0">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s" s="0">
+        <v>627</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>628</v>
+      </c>
+      <c r="E57" t="s" s="0">
+        <v>629</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.81640625"/>
+    <col min="2" max="2" customWidth="true" width="20.90625"/>
+    <col min="3" max="3" customWidth="true" width="23.453125"/>
+    <col min="4" max="4" customWidth="true" width="31.36328125"/>
+    <col min="5" max="5" customWidth="true" width="22.26953125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>323</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>569</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>571</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>573</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>575</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>577</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>579</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>581</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>583</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>585</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>587</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>589</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>591</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>593</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>595</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>597</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -9919,7 +11581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F273D65-64CD-4DA6-A7CB-CBDD420D1D4A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
s2s & purchase Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelResultsFolder/purchaseResults.xlsx
+++ b/src/test/resources/ExcelResultsFolder/purchaseResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\eclipse-workspace\integrationApiUiTesting\src\test\resources\ExcelResultsFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA7FEFD-DD16-43B3-9BF0-30AD70732F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7770E359-6076-47EE-B029-6203A431515D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmailData" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="598">
   <si>
     <t>CardNumber</t>
   </si>
@@ -1826,13 +1826,37 @@
   <si>
     <t>2026-01-09 12:26:58</t>
   </si>
+  <si>
+    <t>6960ba0d5a39512d3852d239</t>
+  </si>
+  <si>
+    <t>2026-01-09 13:49:37</t>
+  </si>
+  <si>
+    <t>INR Master</t>
+  </si>
+  <si>
+    <t>6965deafdaf29e91e691d0fa</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>2026-01-13 11:27:29</t>
+  </si>
+  <si>
+    <t>6965df1bdaf29e91e691d414</t>
+  </si>
+  <si>
+    <t>2026-01-13 11:29:17</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1897,13 +1921,67 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1918,7 +1996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1981,6 +2059,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2286,7 +2382,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2531,7 +2627,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="C64" sqref="C64"/>
@@ -3738,7 +3834,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:7">
       <c r="A69" t="s" s="0">
         <v>570</v>
       </c>
@@ -3761,7 +3857,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:7">
       <c r="A70" t="s" s="0">
         <v>570</v>
       </c>
@@ -3784,7 +3880,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:7">
       <c r="A71" t="s" s="0">
         <v>377</v>
       </c>
@@ -3807,7 +3903,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:7">
       <c r="A72" t="s" s="0">
         <v>377</v>
       </c>
@@ -3830,7 +3926,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:7">
       <c r="A73" t="s" s="0">
         <v>377</v>
       </c>
@@ -3853,7 +3949,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:7">
       <c r="A74" t="s" s="0">
         <v>377</v>
       </c>
@@ -3876,7 +3972,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:7">
       <c r="A75" t="s" s="0">
         <v>377</v>
       </c>
@@ -3897,6 +3993,81 @@
       </c>
       <c r="G75" t="s" s="0">
         <v>589</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s" s="0">
+        <v>377</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C76" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D76" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="E76" t="s" s="0">
+        <v>590</v>
+      </c>
+      <c r="F76" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="G76" t="s" s="0">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>592</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="C77" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D77" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="E77" t="s" s="0">
+        <v>593</v>
+      </c>
+      <c r="F77" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="G77" t="s" s="0">
+        <v>594</v>
+      </c>
+      <c r="H77" t="s" s="0">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>592</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="C78" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="E78" t="s" s="0">
+        <v>596</v>
+      </c>
+      <c r="F78" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="G78" t="s" s="0">
+        <v>594</v>
+      </c>
+      <c r="H78" t="s" s="0">
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -5185,14 +5356,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView topLeftCell="C96" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="23.453125"/>
-    <col min="4" max="4" customWidth="true" width="65.36328125"/>
+    <col min="4" max="4" customWidth="true" width="72.26953125"/>
     <col min="5" max="5" customWidth="true" width="36.7265625"/>
     <col min="6" max="6" customWidth="true" width="19.08984375"/>
     <col min="7" max="7" customWidth="true" width="21.54296875"/>
@@ -7832,7 +8003,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:7">
       <c r="A121" t="s" s="0">
         <v>6</v>
       </c>
@@ -7855,7 +8026,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:7">
       <c r="A122" t="s" s="0">
         <v>6</v>
       </c>
@@ -7887,8 +8058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95DD057-E530-49CE-8A96-15C01556F9C0}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>